<commit_message>
acomodando para la entrega
</commit_message>
<xml_diff>
--- a/Defect Report/DF-001.xlsx
+++ b/Defect Report/DF-001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igu/Documents/UADE/Testing de aplicacioones /TestingAplicaciones-TPO/TestingAplicaciones--IDK--TPO/Defect Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\GitHub\TestingAplicaciones--Jarron-Shang--TPO\Defect Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6EB62-A07A-9F49-80A6-B6F1D7AAB026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A483E36-64E7-4D80-95BB-5B4677ECD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="940" windowWidth="28320" windowHeight="17440" xr2:uid="{106BD81D-11FA-8843-B189-D66095D72D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{106BD81D-11FA-8843-B189-D66095D72D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -95,19 +95,22 @@
     <t xml:space="preserve">Intentamos en varias cuentas y sucede en todas. Esto vuelve a la pagina altamente vulnerable </t>
   </si>
   <si>
-    <t>No diferencia mail DF-002</t>
-  </si>
-  <si>
-    <t>Al registrarse nuevamente en la pagina, se puede utilizar el mismo mail para varias cuentas</t>
-  </si>
-  <si>
-    <t>3- Click en "Register here"</t>
-  </si>
-  <si>
-    <t>4- Completar formulario con el con mail ya ingresado</t>
-  </si>
-  <si>
     <t>Cuenta bloqueada, ingresar al mail para blanquear/cambiar el password</t>
+  </si>
+  <si>
+    <t>Se pueden intentar logear DF-001</t>
+  </si>
+  <si>
+    <t>Al logearse en la cuenta e ingresar mal el password, la pagina identifica que el password es invalido pero te deja intentarlo infinitas veces</t>
+  </si>
+  <si>
+    <t>3- Click en "Log in"</t>
+  </si>
+  <si>
+    <t>4-Ingresar mail valido y password random</t>
+  </si>
+  <si>
+    <t>5-Re intentar infinitas veces.</t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -671,33 +674,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FC200F-4075-6B46-A376-DD80D7FB49CE}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" customWidth="1"/>
+    <col min="2" max="2" width="75.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
@@ -705,33 +708,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
@@ -739,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -747,13 +756,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
@@ -761,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>8</v>
       </c>
@@ -769,7 +778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
@@ -781,7 +790,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>11</v>
       </c>

</xml_diff>